<commit_message>
added TG pojo class and and tdd
</commit_message>
<xml_diff>
--- a/test_data/ReadData.xlsx
+++ b/test_data/ReadData.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="25380" windowHeight="12660"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -43,55 +46,705 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -281,20 +934,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="2" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="3.14285714285714" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -308,35 +971,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" customHeight="1" spans="1:4">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="3" customHeight="1" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>